<commit_message>
update the excel list sheet
</commit_message>
<xml_diff>
--- a/admin_panel/form_list_checkbox_automation.xlsx
+++ b/admin_panel/form_list_checkbox_automation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\admin_panel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E4507A-33C2-4514-8C0B-40BBC801F2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDD3393-48A3-4C51-86EC-B4D7C34D0998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Form Name</t>
   </si>
@@ -103,6 +103,30 @@
   </si>
   <si>
     <t>24. Add New IP</t>
+  </si>
+  <si>
+    <t>25. Add new (block app CRC)</t>
+  </si>
+  <si>
+    <t>26. Add new  (signup balcklist domain)</t>
+  </si>
+  <si>
+    <t>27. Add Server Lock Schedule</t>
+  </si>
+  <si>
+    <t>28. Application &amp; Variable Settings</t>
+  </si>
+  <si>
+    <t>29. Add New Event Code</t>
+  </si>
+  <si>
+    <t>30. Add Event Actions</t>
+  </si>
+  <si>
+    <t>31. Add New PIN Batch (batch subscription)</t>
+  </si>
+  <si>
+    <t>32.Add sub-event code</t>
   </si>
 </sst>
 </file>
@@ -124,7 +148,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,8 +161,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -161,14 +197,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -451,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,7 +548,7 @@
     <col min="1" max="1" width="53.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,144 +556,249 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D2" s="3"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="B4" s="7"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="B5" s="7"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="B6" s="7"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="B7" s="7"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="B10" s="7"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="B11" s="7"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="B12" s="7"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="B13" s="7"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="B14" s="7"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="B15" s="7"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="B16" s="6"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="B17" s="7"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="B18" s="7"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="B19" s="7"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+      <c r="B20" s="7"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+      <c r="B21" s="7"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+      <c r="B22" s="7"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+      <c r="B23" s="7"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
+      <c r="B24" s="7"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="7"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="7"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="E30" s="7"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="E33" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>